<commit_message>
add Lecture 10 data
</commit_message>
<xml_diff>
--- a/files/QT/Lecture_10.xlsx
+++ b/files/QT/Lecture_10.xlsx
@@ -19,12 +19,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Inflation France </t>
   </si>
   <si>
     <t>Unemployment Rate</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X-X_bar</t>
+  </si>
+  <si>
+    <t>Y-Y_bar</t>
+  </si>
+  <si>
+    <t>Covariance</t>
+  </si>
+  <si>
+    <t>Variance of X</t>
+  </si>
+  <si>
+    <t>Variance of Y</t>
+  </si>
+  <si>
+    <t>a =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b = </t>
+  </si>
+  <si>
+    <t>nb of obs</t>
+  </si>
+  <si>
+    <t>R2 =</t>
+  </si>
+  <si>
+    <t>Y_hat - Y_bar</t>
   </si>
 </sst>
 </file>
@@ -73,8 +112,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -86,16 +129,228 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inflation France </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.498734488188976"/>
+                  <c:y val="-0.626395450568679"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2100222552"/>
+        <c:axId val="2100221128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2100222552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2100221128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2100221128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2100222552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,94 +675,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="1" spans="1:9">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2011</v>
       </c>
       <c r="B3" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="C3" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C3" s="1">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <f>B3-B$10</f>
+        <v>-0.74999999999999822</v>
+      </c>
+      <c r="E3">
+        <f>C3-C$10</f>
+        <v>1.2166666666666666</v>
+      </c>
+      <c r="F3">
+        <f>B3*$I$7+$I$8-$C$10</f>
+        <v>1.4416167664670592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2012</v>
       </c>
       <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C4" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="0">B4-B$10</f>
+        <v>-0.14999999999999858</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E8" si="1">C4-C$10</f>
+        <v>1.1166666666666669</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F8" si="2">B4*$I$7+$I$8-$C$10</f>
+        <v>0.28832335329340952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>2013</v>
       </c>
       <c r="B5" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.25000000000000178</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>-8.3333333333333259E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>-0.4805389221556926</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>2014</v>
       </c>
       <c r="B6" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.6</v>
       </c>
-      <c r="C6" s="1">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.25000000000000178</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>-0.48333333333333328</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>-0.4805389221556926</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>2015</v>
       </c>
       <c r="B7" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.1</v>
       </c>
-      <c r="C7" s="1">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.35000000000000142</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>-0.98333333333333328</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>-0.67275449101796991</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f>E10/E11</f>
+        <v>-1.9221556886227547</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>2016</v>
       </c>
       <c r="B8" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.3</v>
       </c>
-      <c r="C8" s="1">
-        <v>9.1999999999999993</v>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000711E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>-0.78333333333333321</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>-9.6107784431141541E-2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <f>C10-I7*B10</f>
+        <v>18.671057884231534</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9">
+        <f>SUMPRODUCT(F3:F8,F3:F8)/6/E12</f>
+        <v>0.67828359404313276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B3:B8)</f>
+        <v>9.1499999999999986</v>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(C3:C8)</f>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <f>SUMPRODUCT(D3:D8,E3:E8)/COUNT(E3:E8)</f>
+        <v>-0.2674999999999999</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.COVARIANCE.P(B3:B8,C3:C8)</f>
+        <v>-0.2674999999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <f>COUNT(E3:E8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f>SUMPRODUCT(D3:D8,D3:D8)/6</f>
+        <v>0.13916666666666661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <f>SUMPRODUCT(E3:E8,E3:E8)/6</f>
+        <v>0.75805555555555559</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>